<commit_message>
1. Using Chrome 2. Added a click event in the login xaml to click in the User ID text box before using the User ID label that appears above in the anchor to type into the User ID field. All this is needed because User ID field is a masked field. 3. Using index 0 thru 4 instead of column names in the add queue item activity.
</commit_message>
<xml_diff>
--- a/WeeklyCitiCreditCardTransactions_GatherDaily/Data/Config.xlsx
+++ b/WeeklyCitiCreditCardTransactions_GatherDaily/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feb79f201121421/UiPATH/WeeklyCreditCardTransactions_GatherDaily/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feb79f201121421/UiPATH/WeeklyCitiCreditCardTransactions_GatherDaily/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="11_6EB4CAF5627EDD8D9FCB0C46929BBE1A46A4B9B1" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{AC2C016C-3544-4304-83DA-6A0ABC8949BB}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="11_6EB4CAF5627EDD8D9FCB0C46929BBE1A46A4B9B1" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{4B4B9A26-80DA-4221-AF55-20F79EB1E959}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>CostcoCiti_Transactions</t>
+  </si>
+  <si>
+    <t>https://online.citi.com/US/ag/mrc/dashboard</t>
+  </si>
+  <si>
+    <t>Citi_Home_URL</t>
   </si>
 </sst>
 </file>
@@ -252,7 +258,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -571,7 +577,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -652,7 +658,12 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>